<commit_message>
Bug fix - manual split select
</commit_message>
<xml_diff>
--- a/source/support/OCECgo_CalExportTemplate.xlsx
+++ b/source/support/OCECgo_CalExportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\PapersWorking\OCECMethod\GitHubRepo\source\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brad\Documents\CodeDevelopment\Projects\OCECgo\source\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BC988B-AE1C-45FE-9C07-082BC9CC18F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A626E91-A0F0-4D5E-A7C8-F05B32E235FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7800" xr2:uid="{B517A4F6-0CBD-4862-A71C-923CC0DC0BD5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B517A4F6-0CBD-4862-A71C-923CC0DC0BD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>"Calibration" NDIR Area [-]</t>
   </si>
@@ -192,6 +192,9 @@
   <si>
     <t>Ambient temperature
 lower limit: [°C]</t>
+  </si>
+  <si>
+    <t># of Data:</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD975AE-5FA1-44C3-8991-CAADDB7C8BC0}">
   <dimension ref="A1:AY50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,7 +1176,7 @@
     <row r="2" spans="1:51" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:51" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="16" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" s="19"/>
     </row>

</xml_diff>